<commit_message>
die Kommantare der einzel Klinik problemlos bekommen werden kann
</commit_message>
<xml_diff>
--- a/Klinikliste.xlsx
+++ b/Klinikliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mel\Documents\Arbeit\Projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taner/Desktop/klinify/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B86CBEE-FD4C-4B91-ABF6-376DC97D9A2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B274294C-BF4E-1C4C-833E-E3084795BA67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CDF4C74C-E155-4ED1-AEE6-0547478CE71C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{CDF4C74C-E155-4ED1-AEE6-0547478CE71C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -299,8 +299,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -320,15 +320,15 @@
   <autoFilter ref="A1:C35" xr:uid="{93FFACCF-88EC-40DD-8F5C-DAF85EAF4E94}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E451B32B-8D07-436F-BE4A-9B074A899C73}" name="Klinikname"/>
-    <tableColumn id="2" xr3:uid="{0D47BC81-6708-4D65-A7C1-CF72DBD4A249}" name="Link Google Maps" dataCellStyle="Link"/>
-    <tableColumn id="3" xr3:uid="{56D45DC0-6A18-4805-A46D-6C6FDF6076C7}" name="Link Klinikbewertungen" dataCellStyle="Link"/>
+    <tableColumn id="2" xr3:uid="{0D47BC81-6708-4D65-A7C1-CF72DBD4A249}" name="Link Google Maps"/>
+    <tableColumn id="3" xr3:uid="{56D45DC0-6A18-4805-A46D-6C6FDF6076C7}" name="Link Klinikbewertungen"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -626,18 +626,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3474B27-FD20-4EE7-B036-C220E6D6A0ED}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -648,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -659,7 +659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -670,7 +670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -681,7 +681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -692,7 +692,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -703,7 +703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -714,7 +714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -736,7 +736,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -747,7 +747,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -758,7 +758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -769,7 +769,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -780,7 +780,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -791,7 +791,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -802,7 +802,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -813,7 +813,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -824,7 +824,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -835,7 +835,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -846,7 +846,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -857,7 +857,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -868,7 +868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -879,7 +879,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -890,7 +890,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -901,7 +901,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -912,43 +912,43 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>

</xml_diff>

<commit_message>
einzel Klinik ohne Problem scrapped
</commit_message>
<xml_diff>
--- a/Klinikliste.xlsx
+++ b/Klinikliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taner/Desktop/klinify/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B274294C-BF4E-1C4C-833E-E3084795BA67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F2F4CA-3197-CD41-B434-2BFBD7987831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{CDF4C74C-E155-4ED1-AEE6-0547478CE71C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{CDF4C74C-E155-4ED1-AEE6-0547478CE71C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -246,10 +246,10 @@
     <t>https://www.klinikbewertungen.de/klinik-forum/erfahrung-mit-krankenhaus-soltau</t>
   </si>
   <si>
-    <t>ttps://www.google.com/maps/place/Heidekreis-Klinikum+GmbH+Krankenhaus+Soltau/@52.9894409,9.847291,15z/data=!3m1!4b1!4m8!1m2!11m1!2s1tsS4C8icZfBtXgqho9ekuv3aB34!3m4!1s0x47b1b</t>
-  </si>
-  <si>
     <t>Krankenhaus Soltau</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Heidekreis-Klinikum+GmbH+Krankenhaus+Soltau/@52.9894409,9.847291,15z/data=!3m1!4b1!4m8!1m2!11m1!2s1tsS4C8icZfBtXgqho9ekuv3aB34!3m4!1s0x47b1b</t>
   </si>
 </sst>
 </file>
@@ -627,13 +627,13 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -903,10 +903,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>72</v>
@@ -992,11 +992,12 @@
     <hyperlink ref="B24" r:id="rId36" xr:uid="{F47C5E1A-4057-4AC5-93C3-7FEB4B58C626}"/>
     <hyperlink ref="C24" r:id="rId37" xr:uid="{2874C5E4-D958-4DC3-9EB9-31FC92022333}"/>
     <hyperlink ref="C25" r:id="rId38" xr:uid="{1004405F-E09A-4241-B110-4D6DFF97D342}"/>
+    <hyperlink ref="B25" r:id="rId39" xr:uid="{76406749-A023-7A4D-B392-7A6B50AF22C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId39"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
   <tableParts count="1">
-    <tablePart r:id="rId40"/>
+    <tablePart r:id="rId41"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>